<commit_message>
Added codelists in Turtle format
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ocorcho/Trabajo/proyectos/2020-Huawei-DevOps/git-public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B3A097-05A1-534E-955C-B8AD806A082D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2D6BD8-0CE3-3A47-B40E-66E1B570CD49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-48360" yWindow="-2500" windowWidth="41760" windowHeight="21200" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="309">
   <si>
     <t>Identifier</t>
   </si>
@@ -908,16 +908,7 @@
     <t>Transmission, MSTP, IPSecVPN</t>
   </si>
   <si>
-    <t>UNUSE, INUSE, APPLY_RECOVERY, READY_FOR_RECOVERY, RECOVERY, NOT_READY_ASSIGN, BROKEN, TO_OFFLINE</t>
-  </si>
-  <si>
     <t>batch, single</t>
-  </si>
-  <si>
-    <t>SHUTOFF, ACTIVE, BUILD, ERROR</t>
-  </si>
-  <si>
-    <t>UNKNOWN, ACTIVE, BUILD, ERROR, HARD_REBOOT, REBOOT, SHUTOFF</t>
   </si>
   <si>
     <t>prePaid, postPaid</t>
@@ -927,12 +918,6 @@
   </si>
   <si>
     <t>database, webcontainer, application, other</t>
-  </si>
-  <si>
-    <t>Master, Slave, Read, Single, DRMaster, DRSlave</t>
-  </si>
-  <si>
-    <t>Master, Slave, MasterAndSlave, Read, Single</t>
   </si>
   <si>
     <t>How a Virtual Server has been created</t>
@@ -960,6 +945,24 @@
   </si>
   <si>
     <t>It identifies the type of database monitor</t>
+  </si>
+  <si>
+    <t>unuse, inuse, apply recovery, ready for recovery, recovery, not ready assign, broken, to offline</t>
+  </si>
+  <si>
+    <t>active, build, error, shutoff</t>
+  </si>
+  <si>
+    <t>master, slave, read, single, DRMaster, DRSlave</t>
+  </si>
+  <si>
+    <t>master, slave, master and slave, read, single</t>
+  </si>
+  <si>
+    <t>active, build, error, shutoff, hard reboot, reboot, unknown</t>
+  </si>
+  <si>
+    <t>active, inactive</t>
   </si>
 </sst>
 </file>
@@ -28592,15 +28595,15 @@
   <dimension ref="A1:D894"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="103.5" customWidth="1"/>
+    <col min="2" max="2" width="78.6640625" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="63.6640625" customWidth="1"/>
+    <col min="4" max="4" width="52.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19" customHeight="1" x14ac:dyDescent="0.15">
@@ -28628,7 +28631,9 @@
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>308</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
@@ -28775,13 +28780,13 @@
         <v>274</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -28789,13 +28794,13 @@
         <v>275</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -28803,13 +28808,13 @@
         <v>276</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -28817,13 +28822,13 @@
         <v>277</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -28831,13 +28836,13 @@
         <v>278</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
@@ -28871,13 +28876,13 @@
         <v>280</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -28885,13 +28890,13 @@
         <v>281</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
@@ -28912,13 +28917,13 @@
         <v>282</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -28926,13 +28931,13 @@
         <v>283</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>